<commit_message>
Setup for datapacks, fixed/added some quests, nerfed spiders
</commit_message>
<xml_diff>
--- a/Quests.xlsx
+++ b/Quests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C077415-F9BA-4524-AC2D-BAAF992DF530}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F23939-4676-4824-97C5-A132A793132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39855" yWindow="3225" windowWidth="26985" windowHeight="15075" activeTab="1" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15885" activeTab="5" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="322">
   <si>
     <t>Quest</t>
   </si>
@@ -438,9 +438,6 @@
     <t>Direct Me The Whey</t>
   </si>
   <si>
-    <t>Assortment of Honeycombs</t>
-  </si>
-  <si>
     <t>80 - 680000</t>
   </si>
   <si>
@@ -967,6 +964,45 @@
   </si>
   <si>
     <t>Bad Kind Of Shroom</t>
+  </si>
+  <si>
+    <t>The Grand Hempening</t>
+  </si>
+  <si>
+    <t>1 Hemp Seed</t>
+  </si>
+  <si>
+    <t>1 Steel Plate</t>
+  </si>
+  <si>
+    <t>Crafting Equipment</t>
+  </si>
+  <si>
+    <t>Full Iron Armor</t>
+  </si>
+  <si>
+    <t>Shield Hero</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>25 uncommon ore</t>
+  </si>
+  <si>
+    <t>Sweet Retribution</t>
+  </si>
+  <si>
+    <t>Honey Shield</t>
+  </si>
+  <si>
+    <t>Assortment of Honeycombs (no quartz)</t>
+  </si>
+  <si>
+    <t>1 Iron Sword 1 crossbow</t>
+  </si>
+  <si>
+    <t>15 uncommon ore</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1116,7 +1152,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1301,6 +1336,12 @@
                 <c:pt idx="22">
                   <c:v>250</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1378,6 +1419,12 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1693,6 +1740,9 @@
                 <c:pt idx="7">
                   <c:v>100</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1725,6 +1775,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3626,6 +3679,9 @@
                 <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="18">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3687,6 +3743,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
@@ -8285,10 +8344,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8397,7 +8456,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>41</v>
@@ -8616,31 +8675,31 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="B12" s="24">
+      <c r="A12" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="B12" s="23">
         <v>20</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>8</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="23">
         <v>8000</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="23">
         <v>200</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="23">
         <v>100</v>
       </c>
     </row>
@@ -8733,7 +8792,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B16" s="8">
         <v>79</v>
@@ -8742,13 +8801,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="G16" s="8">
         <v>4000</v>
@@ -8762,7 +8821,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B17" s="8">
         <v>80</v>
@@ -8774,10 +8833,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>233</v>
       </c>
       <c r="G17" s="8">
         <v>25000</v>
@@ -8789,12 +8848,12 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B18" s="8">
         <v>81</v>
@@ -8806,10 +8865,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G18" s="8">
         <v>2000000</v>
@@ -8823,7 +8882,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B19" s="8">
         <v>82</v>
@@ -8835,10 +8894,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G19" s="8">
         <v>2000000</v>
@@ -8852,7 +8911,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B20" s="8">
         <v>83</v>
@@ -8864,10 +8923,10 @@
         <v>13</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G20" s="8">
         <v>2000000</v>
@@ -8881,7 +8940,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B21" s="8">
         <v>84</v>
@@ -8893,10 +8952,10 @@
         <v>13</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G21" s="8">
         <v>2000000</v>
@@ -8910,7 +8969,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B22" s="8">
         <v>85</v>
@@ -8922,10 +8981,10 @@
         <v>13</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G22" s="8">
         <v>2000000</v>
@@ -8939,7 +8998,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B23" s="8">
         <v>86</v>
@@ -8951,10 +9010,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G23" s="8">
         <v>2000000</v>
@@ -8967,32 +9026,90 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B24" s="8">
+        <v>95</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B24" s="18">
+      <c r="F24" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H24" s="8">
+        <v>250</v>
+      </c>
+      <c r="I24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B25" s="8">
+        <v>109</v>
+      </c>
+      <c r="C25" s="8">
+        <v>6</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G25" s="8">
+        <v>3000</v>
+      </c>
+      <c r="H25" s="8">
+        <v>100</v>
+      </c>
+      <c r="I25" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="B26" s="18">
+        <v>110</v>
+      </c>
+      <c r="C26" s="18">
         <v>95</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="G24" s="18">
-        <v>1000</v>
-      </c>
-      <c r="H24" s="18">
+      <c r="D26" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="G26" s="18">
+        <v>1500</v>
+      </c>
+      <c r="H26" s="18">
         <v>250</v>
       </c>
-      <c r="I24" s="23">
-        <v>0</v>
+      <c r="I26" s="22">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -9012,8 +9129,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A8:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9184,7 +9301,7 @@
         <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>319</v>
       </c>
       <c r="F6" t="s">
         <v>33</v>
@@ -9232,7 +9349,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2">
         <v>45</v>
@@ -9244,10 +9361,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="G8" s="9">
         <f xml:space="preserve"> 1.5 *35000</f>
@@ -9261,38 +9378,67 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="2">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="7">
-        <v>46</v>
-      </c>
-      <c r="C9" s="7">
-        <v>45</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="G9" s="22">
+      <c r="F9" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G9" s="9">
         <f xml:space="preserve"> 1.5 *37500</f>
         <v>56250</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="2">
         <v>100</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="2">
         <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="B10" s="18">
+        <v>111</v>
+      </c>
+      <c r="C10" s="18">
+        <v>14</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="G10" s="7">
+        <v>60000</v>
+      </c>
+      <c r="H10" s="18">
+        <v>150</v>
+      </c>
+      <c r="I10" s="18">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -9309,7 +9455,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9537,7 +9683,7 @@
         <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G8">
         <v>87500</v>
@@ -9638,7 +9784,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" s="2">
         <v>48</v>
@@ -9650,10 +9796,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G12" s="2">
         <f xml:space="preserve"> 3 * 35000</f>
@@ -9668,7 +9814,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" s="2">
         <v>49</v>
@@ -9680,10 +9826,10 @@
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G13" s="2">
         <f xml:space="preserve"> 3 * 25000</f>
@@ -9698,7 +9844,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
@@ -9710,10 +9856,10 @@
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G14" s="2">
         <f xml:space="preserve"> 3 * 30000</f>
@@ -9728,7 +9874,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B15" s="2">
         <v>51</v>
@@ -9740,10 +9886,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G15" s="2">
         <f xml:space="preserve"> 3 * 32500</f>
@@ -9758,7 +9904,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="2">
         <v>52</v>
@@ -9770,10 +9916,10 @@
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="G16" s="2">
         <f xml:space="preserve"> 3 * 35000</f>
@@ -9788,7 +9934,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="2">
         <v>53</v>
@@ -9800,10 +9946,10 @@
         <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G17" s="2">
         <f xml:space="preserve"> 3 * 30000</f>
@@ -9816,12 +9962,12 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="2">
         <v>54</v>
@@ -9833,10 +9979,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G18" s="2">
         <f xml:space="preserve"> 3 * 35000</f>
@@ -9851,22 +9997,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="7">
         <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G19" s="7">
         <f xml:space="preserve"> 3 * 100000</f>
@@ -9894,7 +10040,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9977,7 +10123,7 @@
         <v>102</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G3">
         <v>500000</v>
@@ -10078,7 +10224,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="2">
         <v>56</v>
@@ -10090,10 +10236,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G7" s="2">
         <v>67500</v>
@@ -10107,7 +10253,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B8" s="2">
         <v>57</v>
@@ -10119,10 +10265,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" s="2">
         <v>75000</v>
@@ -10136,7 +10282,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="2">
         <v>58</v>
@@ -10148,10 +10294,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G9" s="2">
         <v>77500</v>
@@ -10165,7 +10311,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" s="2">
         <v>59</v>
@@ -10177,10 +10323,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G10" s="2">
         <v>70000</v>
@@ -10194,7 +10340,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="2">
         <v>60</v>
@@ -10206,10 +10352,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G11" s="2">
         <v>100000</v>
@@ -10223,7 +10369,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B12" s="18">
         <v>107</v>
@@ -10235,10 +10381,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>295</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>296</v>
       </c>
       <c r="G12" s="18">
         <v>50000</v>
@@ -10252,7 +10398,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -10270,7 +10416,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10338,7 +10484,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="2">
         <v>41</v>
@@ -10367,7 +10513,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B4" s="2">
         <v>61</v>
@@ -10379,10 +10525,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G4" s="2">
         <v>175000</v>
@@ -10396,7 +10542,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="2">
         <v>62</v>
@@ -10408,10 +10554,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G5" s="2">
         <v>250000</v>
@@ -10425,7 +10571,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="2">
         <v>63</v>
@@ -10437,10 +10583,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" s="2">
         <v>300000</v>
@@ -10454,7 +10600,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" s="2">
         <v>64</v>
@@ -10466,10 +10612,10 @@
         <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G7" s="2">
         <v>275000</v>
@@ -10483,7 +10629,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" s="2">
         <v>65</v>
@@ -10495,10 +10641,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G8" s="2">
         <v>325000</v>
@@ -10512,7 +10658,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9" s="2">
         <v>66</v>
@@ -10524,10 +10670,10 @@
         <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G9" s="2">
         <v>450000</v>
@@ -10541,7 +10687,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2">
         <v>67</v>
@@ -10553,10 +10699,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G10" s="2">
         <v>200000</v>
@@ -10570,7 +10716,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="2">
         <v>68</v>
@@ -10582,10 +10728,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G11" s="2">
         <v>225000</v>
@@ -10599,7 +10745,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B12" s="2">
         <v>69</v>
@@ -10611,10 +10757,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G12" s="2">
         <v>250000</v>
@@ -10628,7 +10774,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2">
         <v>70</v>
@@ -10640,10 +10786,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G13" s="2">
         <v>200000</v>
@@ -10657,7 +10803,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="2">
         <v>71</v>
@@ -10669,10 +10815,10 @@
         <v>49</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G14" s="2">
         <v>275000</v>
@@ -10686,7 +10832,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B15" s="2">
         <v>72</v>
@@ -10698,10 +10844,10 @@
         <v>49</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G15" s="2">
         <v>325000</v>
@@ -10715,7 +10861,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="2">
         <v>73</v>
@@ -10727,10 +10873,10 @@
         <v>49</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G16" s="2">
         <v>425000</v>
@@ -10744,7 +10890,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="2">
         <v>74</v>
@@ -10756,10 +10902,10 @@
         <v>49</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G17" s="2">
         <v>550000</v>
@@ -10771,12 +10917,12 @@
         <v>250</v>
       </c>
       <c r="K17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="2">
         <v>75</v>
@@ -10788,10 +10934,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G18" s="2">
         <v>400000</v>
@@ -10805,7 +10951,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19" s="2">
         <v>76</v>
@@ -10817,10 +10963,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="G19" s="2">
         <v>500000</v>
@@ -10834,22 +10980,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="14">
         <v>77</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G20" s="14">
         <v>250000</v>
@@ -10876,8 +11022,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10916,7 +11062,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="2">
         <v>78</v>
@@ -10928,7 +11074,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>33</v>
@@ -10945,7 +11091,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B3" s="2">
         <v>97</v>
@@ -10957,10 +11103,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="2">
         <v>625000</v>
@@ -10974,7 +11120,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="2">
         <v>98</v>
@@ -10986,10 +11132,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G4" s="2">
         <v>625000</v>
@@ -11003,7 +11149,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="2">
         <v>99</v>
@@ -11015,10 +11161,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G5" s="2">
         <v>625000</v>
@@ -11032,7 +11178,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B6" s="2">
         <v>100</v>
@@ -11044,10 +11190,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G6" s="2">
         <v>625000</v>
@@ -11061,7 +11207,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" s="2">
         <v>101</v>
@@ -11073,10 +11219,10 @@
         <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G7" s="8">
         <v>500000</v>
@@ -11090,7 +11236,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B8" s="2">
         <v>102</v>
@@ -11102,10 +11248,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G8" s="8">
         <v>500000</v>
@@ -11119,7 +11265,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B9" s="2">
         <v>103</v>
@@ -11131,10 +11277,10 @@
         <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G9" s="8">
         <v>500000</v>
@@ -11148,7 +11294,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B10" s="2">
         <v>104</v>
@@ -11160,10 +11306,10 @@
         <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G10" s="8">
         <v>500000</v>
@@ -11177,7 +11323,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B11" s="2">
         <v>105</v>
@@ -11189,10 +11335,10 @@
         <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G11" s="8">
         <v>500000</v>
@@ -11206,7 +11352,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B12" s="2">
         <v>106</v>
@@ -11218,10 +11364,10 @@
         <v>49</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G12" s="8">
         <v>500000</v>
@@ -11235,22 +11381,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="7">
         <v>20</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G13" s="18">
         <v>1000000</v>
@@ -11264,7 +11410,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -11279,10 +11425,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11341,10 +11487,10 @@
       <c r="G2" s="4">
         <v>1500</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="24">
         <v>50</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="24">
         <v>150</v>
       </c>
     </row>
@@ -11370,10 +11516,10 @@
       <c r="G3" s="4">
         <v>1000</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="24">
         <v>0</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="24">
         <v>150</v>
       </c>
     </row>
@@ -11399,16 +11545,16 @@
       <c r="G4" s="4">
         <v>4000</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="24">
         <v>100</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="24">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="4">
         <v>47</v>
@@ -11420,18 +11566,18 @@
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>210</v>
       </c>
       <c r="G5" s="4">
         <v>10000</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <v>150</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>150</v>
       </c>
     </row>
@@ -11457,10 +11603,10 @@
       <c r="G6" s="5">
         <v>500</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <v>0</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>100</v>
       </c>
     </row>
@@ -11486,10 +11632,10 @@
       <c r="G7" s="5">
         <v>1000</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <v>50</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>100</v>
       </c>
     </row>
@@ -11515,10 +11661,10 @@
       <c r="G8" s="5">
         <v>2000</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="25">
         <v>100</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="25">
         <v>100</v>
       </c>
     </row>
@@ -11544,10 +11690,10 @@
       <c r="G9" s="5">
         <v>4000</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="25">
         <v>150</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="25">
         <v>100</v>
       </c>
     </row>
@@ -11573,16 +11719,16 @@
       <c r="G10" s="5">
         <v>21000</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="25">
         <v>200</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="25">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11" s="17">
         <v>87</v>
@@ -11594,24 +11740,24 @@
         <v>7</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G11" s="17">
         <v>500</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="26">
         <v>0</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B12" s="17">
         <v>88</v>
@@ -11623,10 +11769,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G12" s="17">
         <v>500</v>
@@ -11640,7 +11786,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="17">
         <v>89</v>
@@ -11652,10 +11798,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G13" s="17">
         <v>500</v>
@@ -11669,7 +11815,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" s="17">
         <v>90</v>
@@ -11681,10 +11827,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G14" s="17">
         <v>500</v>
@@ -11698,7 +11844,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B15" s="17">
         <v>91</v>
@@ -11707,13 +11853,13 @@
         <v>90</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G15" s="17">
         <v>500</v>
@@ -11727,7 +11873,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B16" s="17">
         <v>92</v>
@@ -11739,10 +11885,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G16" s="17">
         <v>500</v>
@@ -11756,7 +11902,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B17" s="17">
         <v>93</v>
@@ -11768,10 +11914,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G17" s="17">
         <v>500</v>
@@ -11783,12 +11929,12 @@
         <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B18" s="17">
         <v>94</v>
@@ -11800,10 +11946,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G18" s="17">
         <v>500</v>
@@ -11816,31 +11962,60 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="B19" s="15">
+      <c r="A19" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="6">
         <v>96</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="6">
         <v>0</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="G19" s="15">
+      <c r="D19" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="G19" s="6">
         <v>500</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="6">
         <v>0</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="15">
+        <v>108</v>
+      </c>
+      <c r="C20" s="15">
+        <v>96</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1000</v>
+      </c>
+      <c r="H20" s="15">
+        <v>50</v>
+      </c>
+      <c r="I20" s="15">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quests Update + Lycanites Disable
</commit_message>
<xml_diff>
--- a/Quests.xlsx
+++ b/Quests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\Craft-to-Exile-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D5F598-6A41-4DC3-88D1-F49AB4704C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6347FDB-E581-4BCE-BAC2-17B5E8C0ADFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="680" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="492">
   <si>
     <t>Quest</t>
   </si>
@@ -1493,22 +1493,31 @@
     <t>dwmh:ocarina</t>
   </si>
   <si>
-    <t>100 Zombies</t>
-  </si>
-  <si>
-    <t>100 Skeletons</t>
-  </si>
-  <si>
-    <t>100 Bees</t>
-  </si>
-  <si>
-    <t>100 Zombie Pigmen</t>
-  </si>
-  <si>
-    <t>50 Endermen</t>
-  </si>
-  <si>
-    <t>50 Wither Skeletons</t>
+    <t>5 Purpur Guardian (end guardian)</t>
+  </si>
+  <si>
+    <t>1 Hirschgeist</t>
+  </si>
+  <si>
+    <t>1 Immortal + 1 Deadbeard</t>
+  </si>
+  <si>
+    <t>5 Rotten Spear Eskimos + 5 Ancient Mummies</t>
+  </si>
+  <si>
+    <t>8 Arachnon</t>
+  </si>
+  <si>
+    <t>5 End Trolls</t>
+  </si>
+  <si>
+    <t>Bufflon Mounts</t>
+  </si>
+  <si>
+    <t>bundle of herbs</t>
+  </si>
+  <si>
+    <t>bufflon saddle</t>
   </si>
 </sst>
 </file>
@@ -1808,10 +1817,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Overworld!$H$2:$H$33</c:f>
+              <c:f>Overworld!$H$2:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1906,6 +1915,9 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1913,10 +1925,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overworld!$I$2:$I$33</c:f>
+              <c:f>Overworld!$I$2:$I$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2012,6 +2024,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11913,10 +11928,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12434,7 +12449,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>230</v>
@@ -12463,7 +12478,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>230</v>
@@ -12491,8 +12506,8 @@
       <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>485</v>
+      <c r="E20" s="18" t="s">
+        <v>484</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>230</v>
@@ -12521,7 +12536,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>230</v>
@@ -12550,7 +12565,7 @@
         <v>13</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>230</v>
@@ -12579,7 +12594,7 @@
         <v>13</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>230</v>
@@ -12852,32 +12867,61 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="8" t="s">
         <v>480</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="8">
         <v>173</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="8">
         <v>95</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="14">
         <v>1000</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="8">
         <v>300</v>
       </c>
-      <c r="I33" s="19">
+      <c r="I33" s="14">
         <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B34" s="7">
+        <v>174</v>
+      </c>
+      <c r="C34" s="7">
+        <v>173</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1500</v>
+      </c>
+      <c r="H34" s="7">
+        <v>300</v>
+      </c>
+      <c r="I34" s="7">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -12898,8 +12942,8 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13230,7 +13274,7 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
@@ -13555,7 +13599,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -14140,7 +14184,7 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -14550,7 +14594,7 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -15096,8 +15140,8 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E12:E13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15703,8 +15747,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16135,7 +16179,7 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I21" sqref="A21:I21"/>
     </sheetView>
   </sheetViews>
@@ -16769,8 +16813,8 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Quest and few mod updates
</commit_message>
<xml_diff>
--- a/Quests.xlsx
+++ b/Quests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\Craft-to-Exile-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6347FDB-E581-4BCE-BAC2-17B5E8C0ADFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5887C892-C6AA-43BE-A02D-78B8E3DA70F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="680" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="680" activeTab="7" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="522">
   <si>
     <t>Quest</t>
   </si>
@@ -86,9 +86,6 @@
     <t>KILL_MOB</t>
   </si>
   <si>
-    <t>3 Zombies</t>
-  </si>
-  <si>
     <t>10 Common Ore</t>
   </si>
   <si>
@@ -638,9 +635,6 @@
     <t>10 Reapers</t>
   </si>
   <si>
-    <t>Where Are The Minutemen?!</t>
-  </si>
-  <si>
     <t>1 chief barbarian 10 barbarian</t>
   </si>
   <si>
@@ -764,9 +758,6 @@
     <t>1 Bucket of Milk</t>
   </si>
   <si>
-    <t>6 Zombies, 2 Skeletons, 1 Creepers</t>
-  </si>
-  <si>
     <t>I Can't Carry Anymore</t>
   </si>
   <si>
@@ -1518,13 +1509,112 @@
   </si>
   <si>
     <t>bufflon saddle</t>
+  </si>
+  <si>
+    <t>2 Zombies</t>
+  </si>
+  <si>
+    <t>4 Zombies, 1 Skeletons, 1 Creepers</t>
+  </si>
+  <si>
+    <t>Home Décor</t>
+  </si>
+  <si>
+    <t>macaw + embellish + crayfish furniture</t>
+  </si>
+  <si>
+    <t>Town Hall</t>
+  </si>
+  <si>
+    <t>It's All MINE!</t>
+  </si>
+  <si>
+    <t>Barbarian Raids</t>
+  </si>
+  <si>
+    <t>2 Iron Sword</t>
+  </si>
+  <si>
+    <t>2 Iron Pickaxe</t>
+  </si>
+  <si>
+    <t>2 Iron Axe</t>
+  </si>
+  <si>
+    <t>Fishy Food</t>
+  </si>
+  <si>
+    <t>Population Density</t>
+  </si>
+  <si>
+    <t>embellishcraft:white_oak_fancy_bed</t>
+  </si>
+  <si>
+    <t>mcwfurnitures:nightstand</t>
+  </si>
+  <si>
+    <t>cfm:white_sofa</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhutcitizen</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhutfisherman</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhutguardtower</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhutuniversity</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhutminer</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhutlumberjack</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhuttownhall</t>
+  </si>
+  <si>
+    <t>16 aquaculture:worm</t>
+  </si>
+  <si>
+    <t>16 minecraft:book</t>
+  </si>
+  <si>
+    <t>64 minecraft:oak_log</t>
+  </si>
+  <si>
+    <t>16 minecraft:cooked_porkchop</t>
+  </si>
+  <si>
+    <t>32 mapperbase:raw_bitumen</t>
+  </si>
+  <si>
+    <t>I'm A Lumberjack And I'm OK</t>
+  </si>
+  <si>
+    <t>Guardians Of The City</t>
+  </si>
+  <si>
+    <t>Getting Schooled</t>
+  </si>
+  <si>
+    <t>Have A Beer</t>
+  </si>
+  <si>
+    <t>minecolonies:blockhuttavern</t>
+  </si>
+  <si>
+    <t>1 epic small currency bag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1570,6 +1660,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1670,7 +1767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1708,9 +1805,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4994,7 +5092,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>150</c:v>
@@ -5046,6 +5144,33 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5066,7 +5191,7 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>100</c:v>
@@ -5115,6 +5240,33 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11930,8 +12082,8 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11976,7 +12128,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -11985,7 +12137,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2">
         <v>250</v>
@@ -12010,11 +12162,11 @@
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="2">
         <v>500</v>
@@ -12028,7 +12180,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -12039,11 +12191,11 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>240</v>
+      <c r="E4" s="39" t="s">
+        <v>490</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2">
         <v>750</v>
@@ -12057,7 +12209,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
@@ -12066,13 +12218,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G5" s="3">
         <v>1000</v>
@@ -12086,7 +12238,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -12098,10 +12250,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2">
         <v>500</v>
@@ -12115,7 +12267,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -12127,10 +12279,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G7" s="2">
         <v>1000</v>
@@ -12144,7 +12296,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -12156,10 +12308,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="G8" s="9">
         <v>2000</v>
@@ -12173,7 +12325,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
@@ -12185,10 +12337,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="G9" s="9">
         <v>3000</v>
@@ -12202,7 +12354,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2">
         <v>8</v>
@@ -12214,10 +12366,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="G10" s="9">
         <v>4500</v>
@@ -12231,7 +12383,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>9</v>
@@ -12243,10 +12395,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="G11" s="9">
         <v>6000</v>
@@ -12260,7 +12412,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B12" s="24">
         <v>20</v>
@@ -12272,10 +12424,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>66</v>
       </c>
       <c r="G12" s="25">
         <v>8000</v>
@@ -12289,7 +12441,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B13" s="6">
         <v>42</v>
@@ -12301,10 +12453,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="G13" s="10">
         <v>2000</v>
@@ -12318,7 +12470,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" s="6">
         <v>43</v>
@@ -12330,10 +12482,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" s="10">
         <v>3000</v>
@@ -12347,7 +12499,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" s="6">
         <v>44</v>
@@ -12359,10 +12511,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="G15" s="10">
         <v>5000</v>
@@ -12376,7 +12528,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B16" s="8">
         <v>79</v>
@@ -12385,13 +12537,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="G16" s="14">
         <v>4000</v>
@@ -12405,7 +12557,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B17" s="8">
         <v>80</v>
@@ -12417,10 +12569,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G17" s="14">
         <v>25000</v>
@@ -12432,12 +12584,12 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B18" s="8">
         <v>81</v>
@@ -12449,10 +12601,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G18" s="14">
         <v>2000000</v>
@@ -12466,7 +12618,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B19" s="8">
         <v>82</v>
@@ -12478,10 +12630,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G19" s="14">
         <v>2000000</v>
@@ -12495,7 +12647,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B20" s="8">
         <v>83</v>
@@ -12507,10 +12659,10 @@
         <v>13</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G20" s="14">
         <v>2000000</v>
@@ -12524,7 +12676,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B21" s="8">
         <v>84</v>
@@ -12536,10 +12688,10 @@
         <v>13</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G21" s="14">
         <v>2000000</v>
@@ -12553,7 +12705,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B22" s="8">
         <v>85</v>
@@ -12565,10 +12717,10 @@
         <v>13</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G22" s="14">
         <v>2000000</v>
@@ -12582,7 +12734,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B23" s="8">
         <v>86</v>
@@ -12594,10 +12746,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G23" s="14">
         <v>2000000</v>
@@ -12611,22 +12763,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B24" s="8">
         <v>95</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G24" s="14">
         <v>1000</v>
@@ -12640,7 +12792,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B25" s="8">
         <v>109</v>
@@ -12652,10 +12804,10 @@
         <v>7</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G25" s="14">
         <v>3000</v>
@@ -12669,7 +12821,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B26" s="8">
         <v>110</v>
@@ -12678,13 +12830,13 @@
         <v>95</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G26" s="14">
         <v>1500</v>
@@ -12698,7 +12850,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B27" s="8">
         <v>114</v>
@@ -12710,10 +12862,10 @@
         <v>7</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G27" s="14">
         <v>1250</v>
@@ -12727,7 +12879,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B28" s="6">
         <v>115</v>
@@ -12739,10 +12891,10 @@
         <v>7</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G28" s="10">
         <v>8000</v>
@@ -12756,7 +12908,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B29" s="6">
         <v>116</v>
@@ -12768,10 +12920,10 @@
         <v>7</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G29" s="10">
         <v>4000</v>
@@ -12785,7 +12937,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B30" s="6">
         <v>162</v>
@@ -12797,7 +12949,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="10">
@@ -12812,7 +12964,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B31" s="8">
         <v>163</v>
@@ -12824,10 +12976,10 @@
         <v>13</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G31" s="14">
         <v>200000</v>
@@ -12840,35 +12992,35 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
-        <v>457</v>
-      </c>
-      <c r="B32" s="38">
+      <c r="A32" s="37" t="s">
+        <v>454</v>
+      </c>
+      <c r="B32" s="37">
         <v>164</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="37">
         <v>5</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="38" t="s">
-        <v>458</v>
-      </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39">
+      <c r="E32" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="F32" s="37"/>
+      <c r="G32" s="38">
         <v>1000</v>
       </c>
-      <c r="H32" s="38">
+      <c r="H32" s="37">
         <v>200</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B33" s="8">
         <v>173</v>
@@ -12880,10 +13032,10 @@
         <v>7</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G33" s="14">
         <v>1000</v>
@@ -12897,7 +13049,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B34" s="7">
         <v>174</v>
@@ -12909,10 +13061,10 @@
         <v>7</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="G34" s="7">
         <v>1500</v>
@@ -12982,7 +13134,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B2" s="2">
         <v>165</v>
@@ -12994,7 +13146,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="18">
@@ -13009,7 +13161,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B3" s="2">
         <v>166</v>
@@ -13021,7 +13173,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="18">
@@ -13036,7 +13188,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B4" s="2">
         <v>167</v>
@@ -13048,7 +13200,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="18">
@@ -13063,7 +13215,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B5" s="2">
         <v>168</v>
@@ -13075,7 +13227,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="18">
@@ -13090,7 +13242,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B6" s="2">
         <v>169</v>
@@ -13102,7 +13254,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="18">
@@ -13117,7 +13269,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B7" s="2">
         <v>170</v>
@@ -13129,7 +13281,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="18">
@@ -13144,7 +13296,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B8" s="2">
         <v>171</v>
@@ -13156,7 +13308,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="18">
@@ -13171,7 +13323,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B9" s="7">
         <v>172</v>
@@ -13183,7 +13335,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="27">
@@ -13275,7 +13427,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13314,7 +13466,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -13323,13 +13475,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="18">
         <f>( 1.5 *11000)/2</f>
@@ -13344,7 +13496,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>11</v>
@@ -13356,10 +13508,10 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
       </c>
       <c r="G3" s="18">
         <f>( 1.5 *16000)/2</f>
@@ -13374,7 +13526,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -13386,10 +13538,10 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
         <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
       </c>
       <c r="G4" s="18">
         <f>( 1.5 *30000)/2</f>
@@ -13404,7 +13556,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>13</v>
@@ -13416,10 +13568,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="18">
         <f>( 1.5 *28000)/2</f>
@@ -13434,7 +13586,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -13443,13 +13595,13 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="18">
         <f>( 1.5 *37500)/2</f>
@@ -13464,7 +13616,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="11">
         <v>15</v>
@@ -13473,13 +13625,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G7" s="26">
         <f>( 1.5 *45000)/2</f>
@@ -13494,7 +13646,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="2">
         <v>45</v>
@@ -13503,13 +13655,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="G8" s="18">
         <f>( 1.5 *35000)/2</f>
@@ -13524,7 +13676,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="2">
         <v>46</v>
@@ -13536,10 +13688,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G9" s="18">
         <f>( 1.5 *37500)/2</f>
@@ -13554,7 +13706,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B10" s="16">
         <v>111</v>
@@ -13563,13 +13715,13 @@
         <v>14</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G10" s="27">
         <v>30000</v>
@@ -13583,7 +13735,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -13639,7 +13791,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>16</v>
@@ -13651,10 +13803,10 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
       </c>
       <c r="G2" s="18">
         <v>26000</v>
@@ -13668,7 +13820,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -13677,13 +13829,13 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="18">
         <v>25000</v>
@@ -13697,7 +13849,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>22</v>
@@ -13706,13 +13858,13 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="18">
         <v>31250</v>
@@ -13726,7 +13878,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5">
         <v>23</v>
@@ -13735,13 +13887,13 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="18">
         <v>37500</v>
@@ -13755,7 +13907,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <v>29</v>
@@ -13767,10 +13919,10 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" s="18">
         <v>32500</v>
@@ -13784,7 +13936,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -13793,13 +13945,13 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
         <v>93</v>
-      </c>
-      <c r="F7" t="s">
-        <v>94</v>
       </c>
       <c r="G7" s="18">
         <v>37500</v>
@@ -13813,7 +13965,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8">
         <v>31</v>
@@ -13825,10 +13977,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G8" s="18">
         <v>43750</v>
@@ -13842,7 +13994,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9">
         <v>32</v>
@@ -13854,10 +14006,10 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G9" s="18">
         <v>75000</v>
@@ -13871,22 +14023,22 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
         <v>97</v>
-      </c>
-      <c r="F10" t="s">
-        <v>98</v>
       </c>
       <c r="G10" s="18">
         <v>46250</v>
@@ -13900,7 +14052,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="12">
         <v>34</v>
@@ -13912,10 +14064,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G11" s="28">
         <v>50000</v>
@@ -13929,7 +14081,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B12" s="2">
         <v>48</v>
@@ -13941,10 +14093,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G12" s="18">
         <f>( 3 * 35000)/2</f>
@@ -13959,7 +14111,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" s="2">
         <v>49</v>
@@ -13971,10 +14123,10 @@
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="18">
         <f>( 3 * 25000)/2</f>
@@ -13989,7 +14141,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
@@ -14001,10 +14153,10 @@
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" s="18">
         <f>( 3 * 30000)/2</f>
@@ -14019,7 +14171,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B15" s="2">
         <v>51</v>
@@ -14031,10 +14183,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="18">
         <f>( 3 * 32500)/2</f>
@@ -14049,7 +14201,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B16" s="2">
         <v>52</v>
@@ -14061,10 +14213,10 @@
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="G16" s="18">
         <f>( 3 * 35000)/2</f>
@@ -14079,7 +14231,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="2">
         <v>53</v>
@@ -14091,10 +14243,10 @@
         <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17" s="18">
         <f>( 3 * 30000)/2</f>
@@ -14107,12 +14259,12 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18" s="2">
         <v>54</v>
@@ -14124,10 +14276,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G18" s="18">
         <f>( 3 * 35000)/2</f>
@@ -14142,22 +14294,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B19" s="7">
         <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G19" s="27">
         <f>( 3 * 100000)/2</f>
@@ -14224,7 +14376,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="18">
         <v>35</v>
@@ -14233,13 +14385,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="18">
         <v>62500</v>
@@ -14253,7 +14405,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="18">
         <v>36</v>
@@ -14265,10 +14417,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G3" s="18">
         <v>250000</v>
@@ -14282,7 +14434,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="18">
         <v>37</v>
@@ -14294,10 +14446,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="18">
         <v>67500</v>
@@ -14311,7 +14463,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="18">
         <v>38</v>
@@ -14323,10 +14475,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>106</v>
       </c>
       <c r="G5" s="18">
         <v>71250</v>
@@ -14340,7 +14492,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B6" s="29">
         <v>39</v>
@@ -14352,10 +14504,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="30">
         <v>75000</v>
@@ -14369,7 +14521,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="9">
         <v>56</v>
@@ -14381,10 +14533,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G7" s="18">
         <v>33750</v>
@@ -14398,7 +14550,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B8" s="9">
         <v>57</v>
@@ -14410,10 +14562,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" s="18">
         <v>37500</v>
@@ -14427,7 +14579,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="9">
         <v>58</v>
@@ -14439,10 +14591,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G9" s="18">
         <v>38750</v>
@@ -14456,7 +14608,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B10" s="9">
         <v>59</v>
@@ -14468,10 +14620,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G10" s="18">
         <v>35000</v>
@@ -14485,7 +14637,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="9">
         <v>60</v>
@@ -14497,10 +14649,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G11" s="18">
         <v>50000</v>
@@ -14514,7 +14666,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B12" s="14">
         <v>107</v>
@@ -14526,10 +14678,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="G12" s="18">
         <v>25000</v>
@@ -14543,7 +14695,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B13" s="19">
         <v>112</v>
@@ -14552,13 +14704,13 @@
         <v>35</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G13" s="27">
         <v>25000</v>
@@ -14576,7 +14728,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -14634,7 +14786,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B2" s="14">
         <v>145</v>
@@ -14643,13 +14795,13 @@
         <v>39</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G2" s="14">
         <v>75000</v>
@@ -14663,7 +14815,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B3" s="14">
         <v>146</v>
@@ -14675,10 +14827,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G3" s="14">
         <v>75500</v>
@@ -14692,7 +14844,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B4" s="14">
         <v>147</v>
@@ -14704,10 +14856,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="G4" s="14">
         <v>76000</v>
@@ -14721,7 +14873,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B5" s="14">
         <v>148</v>
@@ -14733,10 +14885,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G5" s="14">
         <v>76000</v>
@@ -14750,7 +14902,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B6" s="14">
         <v>149</v>
@@ -14762,10 +14914,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G6" s="14">
         <v>76500</v>
@@ -14779,7 +14931,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B7" s="14">
         <v>150</v>
@@ -14791,10 +14943,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G7" s="14">
         <v>76000</v>
@@ -14808,7 +14960,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B8" s="14">
         <v>151</v>
@@ -14820,10 +14972,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G8" s="14">
         <v>76500</v>
@@ -14837,22 +14989,22 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B9" s="14">
         <v>152</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G9" s="14">
         <v>78500</v>
@@ -14866,7 +15018,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B10" s="14">
         <v>153</v>
@@ -14878,10 +15030,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G10" s="14">
         <v>100000</v>
@@ -14895,7 +15047,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B11" s="14">
         <v>154</v>
@@ -14907,7 +15059,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14">
@@ -14922,7 +15074,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B12" s="14">
         <v>155</v>
@@ -14934,10 +15086,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G12" s="14">
         <v>65500</v>
@@ -14951,7 +15103,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B13" s="14">
         <v>156</v>
@@ -14963,10 +15115,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G13" s="14">
         <v>66000</v>
@@ -14980,7 +15132,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B14" s="14">
         <v>157</v>
@@ -14992,10 +15144,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G14" s="14">
         <v>65500</v>
@@ -15009,7 +15161,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B15" s="14">
         <v>158</v>
@@ -15021,10 +15173,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="G15" s="14">
         <v>66000</v>
@@ -15038,7 +15190,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B16" s="14">
         <v>159</v>
@@ -15050,10 +15202,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G16" s="14">
         <v>66500</v>
@@ -15067,7 +15219,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B17" s="14">
         <v>160</v>
@@ -15079,10 +15231,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="G17" s="14">
         <v>66500</v>
@@ -15094,12 +15246,12 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B18" s="35">
         <v>161</v>
@@ -15111,7 +15263,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F18" s="36"/>
       <c r="G18" s="35">
@@ -15180,7 +15332,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -15189,13 +15341,13 @@
         <v>153</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="18">
         <v>77500</v>
@@ -15209,7 +15361,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3" s="2">
         <v>41</v>
@@ -15218,13 +15370,13 @@
         <v>153</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="18">
         <v>77500</v>
@@ -15238,7 +15390,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2">
         <v>61</v>
@@ -15250,10 +15402,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G4" s="18">
         <v>87500</v>
@@ -15267,7 +15419,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2">
         <v>62</v>
@@ -15276,13 +15428,13 @@
         <v>61</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G5" s="18">
         <v>125000</v>
@@ -15296,7 +15448,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="2">
         <v>63</v>
@@ -15308,10 +15460,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G6" s="18">
         <v>150000</v>
@@ -15325,7 +15477,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="2">
         <v>64</v>
@@ -15334,13 +15486,13 @@
         <v>62</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G7" s="18">
         <v>137500</v>
@@ -15354,7 +15506,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="2">
         <v>65</v>
@@ -15363,13 +15515,13 @@
         <v>64</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G8" s="18">
         <v>162500</v>
@@ -15383,7 +15535,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="2">
         <v>66</v>
@@ -15392,13 +15544,13 @@
         <v>65</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G9" s="18">
         <v>225000</v>
@@ -15412,7 +15564,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="2">
         <v>67</v>
@@ -15424,10 +15576,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G10" s="18">
         <v>100000</v>
@@ -15441,7 +15593,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="2">
         <v>68</v>
@@ -15453,10 +15605,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G11" s="18">
         <v>112500</v>
@@ -15470,7 +15622,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B12" s="2">
         <v>69</v>
@@ -15482,10 +15634,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G12" s="18">
         <v>125000</v>
@@ -15499,7 +15651,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B13" s="2">
         <v>70</v>
@@ -15511,10 +15663,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G13" s="18">
         <v>100000</v>
@@ -15528,7 +15680,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="2">
         <v>71</v>
@@ -15537,13 +15689,13 @@
         <v>70</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14" s="18">
         <v>137500</v>
@@ -15557,7 +15709,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B15" s="2">
         <v>72</v>
@@ -15566,13 +15718,13 @@
         <v>71</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G15" s="18">
         <v>162500</v>
@@ -15586,7 +15738,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" s="2">
         <v>73</v>
@@ -15595,13 +15747,13 @@
         <v>72</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G16" s="18">
         <v>212500</v>
@@ -15615,7 +15767,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="2">
         <v>74</v>
@@ -15624,13 +15776,13 @@
         <v>73</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G17" s="18">
         <v>275000</v>
@@ -15642,12 +15794,12 @@
         <v>250</v>
       </c>
       <c r="K17" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="2">
         <v>75</v>
@@ -15659,10 +15811,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G18" s="18">
         <v>200000</v>
@@ -15676,7 +15828,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B19" s="2">
         <v>76</v>
@@ -15688,10 +15840,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="G19" s="18">
         <v>250000</v>
@@ -15705,22 +15857,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B20" s="13">
         <v>77</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D20" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G20" s="32">
         <v>125000</v>
@@ -15787,7 +15939,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" s="2">
         <v>78</v>
@@ -15796,13 +15948,13 @@
         <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="18">
         <v>225000</v>
@@ -15816,7 +15968,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B3" s="2">
         <v>97</v>
@@ -15828,10 +15980,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G3" s="18">
         <v>312500</v>
@@ -15845,7 +15997,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B4" s="2">
         <v>98</v>
@@ -15857,10 +16009,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G4" s="18">
         <v>312500</v>
@@ -15874,7 +16026,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B5" s="2">
         <v>99</v>
@@ -15886,10 +16038,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G5" s="18">
         <v>312500</v>
@@ -15903,7 +16055,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B6" s="2">
         <v>100</v>
@@ -15915,10 +16067,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G6" s="18">
         <v>312500</v>
@@ -15932,7 +16084,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B7" s="2">
         <v>101</v>
@@ -15941,13 +16093,13 @@
         <v>78</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G7" s="18">
         <v>250000</v>
@@ -15961,7 +16113,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B8" s="2">
         <v>102</v>
@@ -15970,13 +16122,13 @@
         <v>101</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G8" s="18">
         <v>250000</v>
@@ -15990,7 +16142,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B9" s="2">
         <v>103</v>
@@ -15999,13 +16151,13 @@
         <v>102</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G9" s="18">
         <v>250000</v>
@@ -16019,7 +16171,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B10" s="2">
         <v>104</v>
@@ -16028,13 +16180,13 @@
         <v>103</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G10" s="18">
         <v>250000</v>
@@ -16048,7 +16200,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B11" s="2">
         <v>105</v>
@@ -16057,13 +16209,13 @@
         <v>104</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G11" s="18">
         <v>250000</v>
@@ -16077,7 +16229,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B12" s="2">
         <v>106</v>
@@ -16086,13 +16238,13 @@
         <v>105</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G12" s="18">
         <v>250000</v>
@@ -16106,22 +16258,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B13" s="2">
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G13" s="18">
         <v>500000</v>
@@ -16135,7 +16287,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B14" s="16">
         <v>113</v>
@@ -16144,10 +16296,10 @@
         <v>20</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="27">
@@ -16162,7 +16314,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -16177,10 +16329,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="A21:I21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16219,7 +16371,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4">
         <v>17</v>
@@ -16231,13 +16383,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1500</v>
+      <c r="G2" s="20">
+        <v>1000</v>
       </c>
       <c r="H2" s="20">
         <v>50</v>
@@ -16248,7 +16400,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4">
         <v>18</v>
@@ -16260,13 +16412,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1000</v>
+        <v>14</v>
+      </c>
+      <c r="G3" s="20">
+        <v>500</v>
       </c>
       <c r="H3" s="20">
         <v>0</v>
@@ -16277,28 +16429,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4">
         <v>19</v>
       </c>
-      <c r="C4" s="4">
-        <v>17</v>
+      <c r="C4" s="20">
+        <v>176</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4000</v>
+      <c r="G4" s="20">
+        <v>1000</v>
       </c>
       <c r="H4" s="20">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I4" s="20">
         <v>150</v>
@@ -16306,36 +16458,36 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>198</v>
+        <v>495</v>
       </c>
       <c r="B5" s="4">
         <v>47</v>
       </c>
-      <c r="C5" s="4">
-        <v>19</v>
+      <c r="C5" s="20">
+        <v>179</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G5" s="20">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="H5" s="20">
         <v>150</v>
       </c>
       <c r="I5" s="20">
-        <v>150</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5">
         <v>24</v>
@@ -16347,10 +16499,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="G6" s="21">
         <v>500</v>
@@ -16364,7 +16516,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="5">
         <v>25</v>
@@ -16376,10 +16528,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="G7" s="21">
         <v>1000</v>
@@ -16393,7 +16545,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="5">
         <v>26</v>
@@ -16405,10 +16557,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="21">
         <v>2000</v>
@@ -16422,7 +16574,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5">
         <v>27</v>
@@ -16434,10 +16586,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="G9" s="21">
         <v>4000</v>
@@ -16451,7 +16603,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="5">
         <v>28</v>
@@ -16460,16 +16612,16 @@
         <v>27</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="G10" s="21">
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="H10" s="21">
         <v>200</v>
@@ -16480,7 +16632,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B11" s="15">
         <v>87</v>
@@ -16492,10 +16644,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G11" s="22">
         <v>500</v>
@@ -16509,7 +16661,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B12" s="15">
         <v>88</v>
@@ -16521,10 +16673,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G12" s="15">
         <v>500</v>
@@ -16538,7 +16690,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B13" s="15">
         <v>89</v>
@@ -16550,10 +16702,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G13" s="15">
         <v>500</v>
@@ -16567,7 +16719,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B14" s="15">
         <v>90</v>
@@ -16579,10 +16731,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G14" s="15">
         <v>500</v>
@@ -16596,7 +16748,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B15" s="15">
         <v>91</v>
@@ -16605,13 +16757,13 @@
         <v>90</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G15" s="15">
         <v>500</v>
@@ -16625,7 +16777,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B16" s="15">
         <v>92</v>
@@ -16637,10 +16789,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G16" s="15">
         <v>500</v>
@@ -16654,7 +16806,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B17" s="15">
         <v>93</v>
@@ -16666,10 +16818,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G17" s="15">
         <v>500</v>
@@ -16681,12 +16833,12 @@
         <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B18" s="15">
         <v>94</v>
@@ -16698,10 +16850,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G18" s="15">
         <v>500</v>
@@ -16715,7 +16867,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B19" s="15">
         <v>117</v>
@@ -16727,10 +16879,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G19" s="15">
         <v>500</v>
@@ -16744,7 +16896,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B20" s="15">
         <v>118</v>
@@ -16756,10 +16908,10 @@
         <v>7</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G20" s="15">
         <v>1000</v>
@@ -16772,32 +16924,302 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
-        <v>329</v>
-      </c>
-      <c r="B21" s="37">
+      <c r="A21" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B21" s="15">
         <v>119</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="15">
         <v>118</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>430</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>431</v>
-      </c>
-      <c r="G21" s="37">
+      <c r="E21" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="G21" s="15">
         <v>1000</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="15">
         <v>300</v>
       </c>
-      <c r="I21" s="37">
+      <c r="I21" s="15">
         <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>491</v>
+      </c>
+      <c r="B22" s="15">
+        <v>175</v>
+      </c>
+      <c r="C22" s="15">
+        <v>91</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="G22" s="15">
+        <v>1000</v>
+      </c>
+      <c r="H22" s="15">
+        <v>200</v>
+      </c>
+      <c r="I22" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="B23" s="4">
+        <v>176</v>
+      </c>
+      <c r="C23" s="4">
+        <v>17</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H23" s="4">
+        <v>100</v>
+      </c>
+      <c r="I23" s="4">
+        <v>150</v>
+      </c>
+      <c r="K23" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B24" s="4">
+        <v>177</v>
+      </c>
+      <c r="C24" s="4">
+        <v>19</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H24" s="4">
+        <v>200</v>
+      </c>
+      <c r="I24" s="4">
+        <v>150</v>
+      </c>
+      <c r="K24" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B25" s="4">
+        <v>178</v>
+      </c>
+      <c r="C25" s="4">
+        <v>177</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H25" s="4">
+        <v>250</v>
+      </c>
+      <c r="I25" s="4">
+        <v>150</v>
+      </c>
+      <c r="K25" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="B26" s="4">
+        <v>179</v>
+      </c>
+      <c r="C26" s="4">
+        <v>19</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="4">
+        <v>150</v>
+      </c>
+      <c r="I26" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B27" s="4">
+        <v>180</v>
+      </c>
+      <c r="C27" s="4">
+        <v>178</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="4">
+        <v>250</v>
+      </c>
+      <c r="I27" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B28" s="4">
+        <v>181</v>
+      </c>
+      <c r="C28" s="4">
+        <v>178</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H28" s="4">
+        <v>300</v>
+      </c>
+      <c r="I28" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B29" s="4">
+        <v>182</v>
+      </c>
+      <c r="C29" s="4">
+        <v>178</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H29" s="4">
+        <v>300</v>
+      </c>
+      <c r="I29" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>519</v>
+      </c>
+      <c r="B30" s="40">
+        <v>183</v>
+      </c>
+      <c r="C30" s="40">
+        <v>182</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>520</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>521</v>
+      </c>
+      <c r="G30" s="40">
+        <v>1500</v>
+      </c>
+      <c r="H30" s="40">
+        <v>350</v>
+      </c>
+      <c r="I30" s="40">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -16853,7 +17275,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B2" s="6">
         <v>96</v>
@@ -16862,13 +17284,13 @@
         <v>134</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G2" s="10">
         <v>1000</v>
@@ -16882,7 +17304,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B3" s="6">
         <v>108</v>
@@ -16894,10 +17316,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G3" s="10">
         <v>1000</v>
@@ -16911,7 +17333,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B4" s="14">
         <v>120</v>
@@ -16921,10 +17343,10 @@
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G4" s="14">
         <v>500</v>
@@ -16938,7 +17360,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B5" s="14">
         <v>121</v>
@@ -16948,10 +17370,10 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G5" s="14">
         <v>500</v>
@@ -16965,7 +17387,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B6" s="14">
         <v>122</v>
@@ -16975,10 +17397,10 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G6" s="14">
         <v>500</v>
@@ -16992,7 +17414,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B7" s="14">
         <v>123</v>
@@ -17002,10 +17424,10 @@
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G7" s="14">
         <v>500</v>
@@ -17019,7 +17441,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B8" s="14">
         <v>124</v>
@@ -17029,10 +17451,10 @@
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G8" s="14">
         <v>500</v>
@@ -17046,7 +17468,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B9" s="14">
         <v>125</v>
@@ -17056,10 +17478,10 @@
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G9" s="14">
         <v>1000</v>
@@ -17073,7 +17495,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B10" s="14">
         <v>126</v>
@@ -17083,10 +17505,10 @@
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G10" s="14">
         <v>1000</v>
@@ -17100,7 +17522,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B11" s="14">
         <v>127</v>
@@ -17110,10 +17532,10 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G11" s="14">
         <v>500</v>
@@ -17127,7 +17549,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B12" s="14">
         <v>128</v>
@@ -17137,7 +17559,7 @@
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
@@ -17152,7 +17574,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B13" s="14">
         <v>129</v>
@@ -17162,7 +17584,7 @@
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14">
@@ -17177,7 +17599,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B14" s="14">
         <v>130</v>
@@ -17187,7 +17609,7 @@
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14">
@@ -17202,7 +17624,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B15" s="14">
         <v>131</v>
@@ -17212,10 +17634,10 @@
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G15" s="14">
         <v>500</v>
@@ -17229,7 +17651,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B16" s="14">
         <v>132</v>
@@ -17239,10 +17661,10 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G16" s="14">
         <v>500</v>
@@ -17256,7 +17678,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B17" s="14">
         <v>133</v>
@@ -17266,7 +17688,7 @@
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14">
@@ -17279,12 +17701,12 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B18" s="14">
         <v>134</v>
@@ -17294,10 +17716,10 @@
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G18" s="14">
         <v>500</v>
@@ -17311,7 +17733,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B19" s="10">
         <v>135</v>
@@ -17321,10 +17743,10 @@
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G19" s="10">
         <v>1000</v>
@@ -17338,7 +17760,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B20" s="10">
         <v>136</v>
@@ -17348,10 +17770,10 @@
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G20" s="10">
         <v>1000</v>
@@ -17365,7 +17787,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B21" s="10">
         <v>137</v>
@@ -17375,7 +17797,7 @@
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10">
@@ -17390,7 +17812,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B22" s="10">
         <v>138</v>
@@ -17400,7 +17822,7 @@
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="10" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10">
@@ -17415,7 +17837,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B23" s="10">
         <v>139</v>
@@ -17425,7 +17847,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="10" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10">
@@ -17440,7 +17862,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B24" s="10">
         <v>140</v>
@@ -17450,10 +17872,10 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="10" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G24" s="10">
         <v>1000</v>
@@ -17467,7 +17889,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B25" s="10">
         <v>141</v>
@@ -17477,10 +17899,10 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="10" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G25" s="10">
         <v>1000</v>
@@ -17494,7 +17916,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B26" s="10">
         <v>142</v>
@@ -17504,10 +17926,10 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="10" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G26" s="10">
         <v>1000</v>
@@ -17521,7 +17943,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B27" s="10">
         <v>143</v>
@@ -17531,10 +17953,10 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="10" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G27" s="10">
         <v>1000</v>
@@ -17548,7 +17970,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B28" s="34">
         <v>144</v>
@@ -17558,10 +17980,10 @@
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="34" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G28" s="34">
         <v>1000</v>

</xml_diff>

<commit_message>
pre terraforged + ftb
</commit_message>
<xml_diff>
--- a/Quests.xlsx
+++ b/Quests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1EE8AA-D51A-431D-B71E-73D988CF7B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754E1D56-BBDB-48BF-B9B9-BADB8C749589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="680" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="16440" tabRatio="680" activeTab="5" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -594,15 +594,9 @@
     <t>64 Rainbow Berries</t>
   </si>
   <si>
-    <t>Source Of Negativity</t>
-  </si>
-  <si>
     <t>1 epic big gear, 1 epic big currency</t>
   </si>
   <si>
-    <t>15 Lobber</t>
-  </si>
-  <si>
     <t>3 Spectre</t>
   </si>
   <si>
@@ -1876,6 +1870,12 @@
   </si>
   <si>
     <t>32 wheat</t>
+  </si>
+  <si>
+    <t>10 Lava Monster</t>
+  </si>
+  <si>
+    <t>Flame On!</t>
   </si>
 </sst>
 </file>
@@ -13406,7 +13406,7 @@
   </sheetPr>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -13487,7 +13487,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
@@ -13516,7 +13516,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>40</v>
@@ -13548,7 +13548,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G5" s="35">
         <v>1500</v>
@@ -13736,7 +13736,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B12" s="9">
         <v>189</v>
@@ -13748,10 +13748,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G12" s="18">
         <v>6750</v>
@@ -13806,7 +13806,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>118</v>
@@ -13852,7 +13852,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B16" s="8">
         <v>79</v>
@@ -13861,13 +13861,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>211</v>
       </c>
       <c r="G16" s="18">
         <v>6000</v>
@@ -13881,7 +13881,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B17" s="8">
         <v>80</v>
@@ -13893,10 +13893,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G17" s="18">
         <v>37500</v>
@@ -13913,7 +13913,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B18" s="8">
         <v>81</v>
@@ -13925,10 +13925,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G18" s="14">
         <v>2000000</v>
@@ -13942,7 +13942,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B19" s="8">
         <v>82</v>
@@ -13954,10 +13954,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G19" s="14">
         <v>2000000</v>
@@ -13971,7 +13971,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B20" s="8">
         <v>83</v>
@@ -13983,10 +13983,10 @@
         <v>13</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G20" s="14">
         <v>2000000</v>
@@ -14000,7 +14000,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B21" s="8">
         <v>84</v>
@@ -14012,10 +14012,10 @@
         <v>13</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G21" s="14">
         <v>2000000</v>
@@ -14029,7 +14029,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B22" s="8">
         <v>85</v>
@@ -14041,10 +14041,10 @@
         <v>13</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G22" s="14">
         <v>2000000</v>
@@ -14058,7 +14058,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B23" s="8">
         <v>86</v>
@@ -14070,10 +14070,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G23" s="14">
         <v>2000000</v>
@@ -14087,7 +14087,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B24" s="8">
         <v>95</v>
@@ -14099,10 +14099,10 @@
         <v>7</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G24" s="18">
         <v>1500</v>
@@ -14116,7 +14116,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B25" s="8">
         <v>109</v>
@@ -14128,10 +14128,10 @@
         <v>7</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G25" s="18">
         <v>4500</v>
@@ -14145,7 +14145,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B26" s="8">
         <v>110</v>
@@ -14154,13 +14154,13 @@
         <v>95</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G26" s="18">
         <v>2250</v>
@@ -14174,7 +14174,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B27" s="8">
         <v>114</v>
@@ -14186,10 +14186,10 @@
         <v>7</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G27" s="18">
         <v>1875</v>
@@ -14203,7 +14203,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B28" s="6">
         <v>115</v>
@@ -14215,10 +14215,10 @@
         <v>7</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G28" s="10">
         <v>8000</v>
@@ -14232,7 +14232,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B29" s="6">
         <v>116</v>
@@ -14244,10 +14244,10 @@
         <v>7</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G29" s="10">
         <v>4000</v>
@@ -14261,7 +14261,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B30" s="6">
         <v>162</v>
@@ -14273,7 +14273,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="10">
@@ -14288,7 +14288,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B31" s="8">
         <v>163</v>
@@ -14300,10 +14300,10 @@
         <v>13</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G31" s="14">
         <v>200000</v>
@@ -14317,7 +14317,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B32" s="33">
         <v>164</v>
@@ -14329,7 +14329,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="37">
@@ -14344,7 +14344,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B33" s="8">
         <v>173</v>
@@ -14356,10 +14356,10 @@
         <v>7</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G33" s="18">
         <v>1500</v>
@@ -14373,7 +14373,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B34" s="2">
         <v>174</v>
@@ -14385,10 +14385,10 @@
         <v>7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G34" s="9">
         <v>2250</v>
@@ -14402,7 +14402,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B35" s="16">
         <v>213</v>
@@ -14414,10 +14414,10 @@
         <v>7</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="G35" s="19">
         <v>4500</v>
@@ -14487,22 +14487,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B2" s="6">
         <v>96</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G2" s="10">
         <v>1000</v>
@@ -14516,7 +14516,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B3" s="6">
         <v>108</v>
@@ -14528,10 +14528,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G3" s="10">
         <v>1000</v>
@@ -14545,7 +14545,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B4" s="14">
         <v>120</v>
@@ -14555,10 +14555,10 @@
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G4" s="14">
         <v>500</v>
@@ -14572,7 +14572,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B5" s="14">
         <v>121</v>
@@ -14582,10 +14582,10 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G5" s="14">
         <v>500</v>
@@ -14599,7 +14599,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B6" s="14">
         <v>122</v>
@@ -14609,10 +14609,10 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G6" s="14">
         <v>500</v>
@@ -14626,7 +14626,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B7" s="14">
         <v>123</v>
@@ -14636,10 +14636,10 @@
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G7" s="14">
         <v>500</v>
@@ -14653,7 +14653,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B8" s="14">
         <v>124</v>
@@ -14663,10 +14663,10 @@
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G8" s="14">
         <v>500</v>
@@ -14680,7 +14680,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B9" s="14">
         <v>125</v>
@@ -14690,10 +14690,10 @@
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G9" s="14">
         <v>1000</v>
@@ -14707,7 +14707,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B10" s="14">
         <v>126</v>
@@ -14717,10 +14717,10 @@
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G10" s="14">
         <v>1000</v>
@@ -14734,7 +14734,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B11" s="14">
         <v>127</v>
@@ -14744,10 +14744,10 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G11" s="14">
         <v>500</v>
@@ -14761,7 +14761,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B12" s="14">
         <v>128</v>
@@ -14771,7 +14771,7 @@
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
@@ -14786,7 +14786,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B13" s="14">
         <v>129</v>
@@ -14796,7 +14796,7 @@
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14">
@@ -14811,7 +14811,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B14" s="14">
         <v>130</v>
@@ -14821,7 +14821,7 @@
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14">
@@ -14836,7 +14836,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B15" s="14">
         <v>131</v>
@@ -14846,10 +14846,10 @@
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G15" s="14">
         <v>500</v>
@@ -14863,7 +14863,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B16" s="14">
         <v>132</v>
@@ -14873,10 +14873,10 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G16" s="14">
         <v>500</v>
@@ -14890,7 +14890,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B17" s="14">
         <v>133</v>
@@ -14900,7 +14900,7 @@
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14">
@@ -14918,7 +14918,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B18" s="14">
         <v>134</v>
@@ -14928,10 +14928,10 @@
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G18" s="14">
         <v>500</v>
@@ -14945,7 +14945,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B19" s="10">
         <v>135</v>
@@ -14955,10 +14955,10 @@
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G19" s="10">
         <v>1000</v>
@@ -14972,7 +14972,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B20" s="10">
         <v>136</v>
@@ -14982,10 +14982,10 @@
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G20" s="10">
         <v>1000</v>
@@ -14999,7 +14999,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B21" s="10">
         <v>137</v>
@@ -15009,7 +15009,7 @@
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10">
@@ -15024,7 +15024,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B22" s="10">
         <v>138</v>
@@ -15034,7 +15034,7 @@
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10">
@@ -15049,7 +15049,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B23" s="10">
         <v>139</v>
@@ -15059,7 +15059,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10">
@@ -15074,7 +15074,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B24" s="10">
         <v>140</v>
@@ -15084,10 +15084,10 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G24" s="10">
         <v>1000</v>
@@ -15101,7 +15101,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B25" s="10">
         <v>141</v>
@@ -15111,10 +15111,10 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G25" s="10">
         <v>1000</v>
@@ -15128,7 +15128,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B26" s="10">
         <v>142</v>
@@ -15138,10 +15138,10 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G26" s="10">
         <v>1000</v>
@@ -15155,7 +15155,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B27" s="10">
         <v>143</v>
@@ -15165,10 +15165,10 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G27" s="10">
         <v>1000</v>
@@ -15182,7 +15182,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B28" s="32">
         <v>144</v>
@@ -15192,10 +15192,10 @@
       </c>
       <c r="D28" s="31"/>
       <c r="E28" s="32" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G28" s="32">
         <v>1000</v>
@@ -15262,7 +15262,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B2" s="2">
         <v>165</v>
@@ -15274,7 +15274,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="18">
@@ -15289,7 +15289,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B3" s="2">
         <v>166</v>
@@ -15301,7 +15301,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="18">
@@ -15316,7 +15316,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B4" s="2">
         <v>167</v>
@@ -15328,7 +15328,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="18">
@@ -15343,7 +15343,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B5" s="2">
         <v>168</v>
@@ -15355,7 +15355,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="18">
@@ -15370,7 +15370,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B6" s="2">
         <v>169</v>
@@ -15382,7 +15382,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="18">
@@ -15397,7 +15397,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B7" s="2">
         <v>170</v>
@@ -15409,7 +15409,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="18">
@@ -15424,7 +15424,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B8" s="2">
         <v>171</v>
@@ -15436,7 +15436,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="18">
@@ -15451,7 +15451,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B9" s="7">
         <v>172</v>
@@ -15463,7 +15463,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="25">
@@ -15606,7 +15606,7 @@
         <v>48</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F2" t="s">
         <v>46</v>
@@ -15636,7 +15636,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F3" t="s">
         <v>50</v>
@@ -15696,7 +15696,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F5" t="s">
         <v>32</v>
@@ -15726,7 +15726,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
@@ -15759,7 +15759,7 @@
         <v>57</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G7" s="24">
         <f>( 1.5 *45000)/2</f>
@@ -15786,7 +15786,7 @@
         <v>48</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>125</v>
@@ -15816,10 +15816,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G9" s="18">
         <f>( 1.5 *37500)/2</f>
@@ -15834,7 +15834,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B10" s="8">
         <v>111</v>
@@ -15843,13 +15843,13 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G10" s="9">
         <v>30000</v>
@@ -15863,7 +15863,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B11" s="8">
         <v>184</v>
@@ -15875,10 +15875,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G11" s="2">
         <v>30000</v>
@@ -15892,7 +15892,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B12" s="8">
         <v>185</v>
@@ -15904,10 +15904,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G12" s="2">
         <v>30500</v>
@@ -15921,7 +15921,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B13" s="16">
         <v>186</v>
@@ -15933,10 +15933,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G13" s="19">
         <v>25000</v>
@@ -15950,7 +15950,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -16196,7 +16196,7 @@
         <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G8" s="18">
         <v>43750</v>
@@ -16283,7 +16283,7 @@
         <v>94</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G11" s="26">
         <v>50000</v>
@@ -16297,7 +16297,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B12" s="2">
         <v>48</v>
@@ -16309,7 +16309,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>127</v>
@@ -16357,7 +16357,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
@@ -16387,7 +16387,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B15" s="2">
         <v>51</v>
@@ -16417,7 +16417,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B16" s="2">
         <v>52</v>
@@ -16475,7 +16475,7 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -16636,7 +16636,7 @@
         <v>95</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G3" s="18">
         <v>250000</v>
@@ -16708,7 +16708,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B6" s="27">
         <v>39</v>
@@ -16720,7 +16720,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>32</v>
@@ -16766,7 +16766,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B8" s="9">
         <v>57</v>
@@ -16824,7 +16824,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B10" s="9">
         <v>59</v>
@@ -16882,7 +16882,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B12" s="14">
         <v>107</v>
@@ -16894,10 +16894,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G12" s="18">
         <v>25000</v>
@@ -16911,7 +16911,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B13" s="14">
         <v>112</v>
@@ -16923,10 +16923,10 @@
         <v>18</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G13" s="9">
         <v>25000</v>
@@ -16940,7 +16940,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B14" s="14">
         <v>187</v>
@@ -16952,10 +16952,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="G14" s="14">
         <v>30000</v>
@@ -16969,7 +16969,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B15" s="19">
         <v>188</v>
@@ -16981,10 +16981,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G15" s="19">
         <v>52500</v>
@@ -16998,7 +16998,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -17056,7 +17056,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B2" s="14">
         <v>145</v>
@@ -17068,10 +17068,10 @@
         <v>18</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G2" s="14">
         <v>75000</v>
@@ -17085,7 +17085,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B3" s="14">
         <v>146</v>
@@ -17097,10 +17097,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G3" s="14">
         <v>75500</v>
@@ -17114,7 +17114,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B4" s="14">
         <v>147</v>
@@ -17126,10 +17126,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G4" s="14">
         <v>76000</v>
@@ -17143,7 +17143,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B5" s="14">
         <v>148</v>
@@ -17155,10 +17155,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G5" s="14">
         <v>76000</v>
@@ -17172,7 +17172,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B6" s="14">
         <v>149</v>
@@ -17184,10 +17184,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G6" s="14">
         <v>76500</v>
@@ -17201,7 +17201,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B7" s="14">
         <v>150</v>
@@ -17213,10 +17213,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G7" s="14">
         <v>76000</v>
@@ -17230,7 +17230,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B8" s="14">
         <v>151</v>
@@ -17242,10 +17242,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G8" s="14">
         <v>76500</v>
@@ -17259,22 +17259,22 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B9" s="14">
         <v>152</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G9" s="14">
         <v>78500</v>
@@ -17288,7 +17288,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B10" s="14">
         <v>153</v>
@@ -17300,10 +17300,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G10" s="14">
         <v>100000</v>
@@ -17317,7 +17317,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B11" s="14">
         <v>154</v>
@@ -17329,7 +17329,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14">
@@ -17344,7 +17344,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B12" s="14">
         <v>155</v>
@@ -17356,10 +17356,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G12" s="14">
         <v>65500</v>
@@ -17373,7 +17373,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B13" s="14">
         <v>156</v>
@@ -17385,10 +17385,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G13" s="14">
         <v>66000</v>
@@ -17402,7 +17402,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B14" s="14">
         <v>157</v>
@@ -17414,10 +17414,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G14" s="14">
         <v>65500</v>
@@ -17431,7 +17431,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B15" s="14">
         <v>158</v>
@@ -17443,10 +17443,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G15" s="14">
         <v>66000</v>
@@ -17460,7 +17460,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B16" s="14">
         <v>159</v>
@@ -17472,10 +17472,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G16" s="14">
         <v>66500</v>
@@ -17489,7 +17489,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B17" s="14">
         <v>160</v>
@@ -17501,10 +17501,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G17" s="14">
         <v>66500</v>
@@ -17516,12 +17516,12 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B18" s="38">
         <v>161</v>
@@ -17533,7 +17533,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="38">
@@ -17548,7 +17548,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B19" s="19">
         <v>190</v>
@@ -17560,10 +17560,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="G19" s="19">
         <v>77000</v>
@@ -17591,8 +17591,8 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17660,7 +17660,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B3" s="2">
         <v>41</v>
@@ -17762,7 +17762,7 @@
         <v>156</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G6" s="18">
         <v>150000</v>
@@ -17849,7 +17849,7 @@
         <v>178</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G9" s="18">
         <v>225000</v>
@@ -17921,7 +17921,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B12" s="2">
         <v>69</v>
@@ -18008,7 +18008,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B15" s="2">
         <v>72</v>
@@ -18093,12 +18093,12 @@
         <v>250</v>
       </c>
       <c r="K17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>183</v>
+        <v>610</v>
       </c>
       <c r="B18" s="2">
         <v>75</v>
@@ -18110,7 +18110,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>185</v>
+        <v>609</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>144</v>
@@ -18127,7 +18127,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B19" s="2">
         <v>76</v>
@@ -18139,10 +18139,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G19" s="18">
         <v>250000</v>
@@ -18156,22 +18156,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B20" s="13">
         <v>77</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G20" s="30">
         <v>125000</v>
@@ -18238,7 +18238,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2">
         <v>78</v>
@@ -18250,7 +18250,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>32</v>
@@ -18267,7 +18267,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3" s="2">
         <v>97</v>
@@ -18279,10 +18279,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G3" s="18">
         <v>312500</v>
@@ -18296,7 +18296,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B4" s="2">
         <v>98</v>
@@ -18308,10 +18308,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G4" s="18">
         <v>312500</v>
@@ -18325,7 +18325,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B5" s="2">
         <v>99</v>
@@ -18337,10 +18337,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G5" s="18">
         <v>312500</v>
@@ -18354,7 +18354,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B6" s="2">
         <v>100</v>
@@ -18366,10 +18366,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G6" s="18">
         <v>312500</v>
@@ -18383,7 +18383,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B7" s="2">
         <v>101</v>
@@ -18395,10 +18395,10 @@
         <v>48</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G7" s="18">
         <v>250000</v>
@@ -18412,7 +18412,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B8" s="2">
         <v>102</v>
@@ -18424,10 +18424,10 @@
         <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G8" s="18">
         <v>250000</v>
@@ -18441,7 +18441,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B9" s="2">
         <v>103</v>
@@ -18453,10 +18453,10 @@
         <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G9" s="18">
         <v>250000</v>
@@ -18470,7 +18470,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B10" s="2">
         <v>104</v>
@@ -18482,10 +18482,10 @@
         <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G10" s="18">
         <v>250000</v>
@@ -18499,7 +18499,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B11" s="2">
         <v>105</v>
@@ -18511,10 +18511,10 @@
         <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G11" s="9">
         <v>250000</v>
@@ -18528,7 +18528,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B12" s="2">
         <v>106</v>
@@ -18540,10 +18540,10 @@
         <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G12" s="9">
         <v>250000</v>
@@ -18557,22 +18557,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B13" s="8">
         <v>191</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="G13" s="14">
         <v>300000</v>
@@ -18586,7 +18586,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B14" s="8">
         <v>192</v>
@@ -18598,7 +18598,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="14">
@@ -18613,7 +18613,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B15" s="7">
         <v>212</v>
@@ -18625,7 +18625,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="19">
@@ -18640,7 +18640,7 @@
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -18697,7 +18697,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B2" s="2">
         <v>193</v>
@@ -18709,10 +18709,10 @@
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G2" s="18">
         <v>375000</v>
@@ -18726,7 +18726,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B3" s="2">
         <v>194</v>
@@ -18738,10 +18738,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G3" s="18">
         <v>350000</v>
@@ -18755,7 +18755,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B4" s="2">
         <v>195</v>
@@ -18767,10 +18767,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G4" s="18">
         <v>365000</v>
@@ -18784,7 +18784,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B5" s="8">
         <v>196</v>
@@ -18796,10 +18796,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G5" s="18">
         <v>375000</v>
@@ -18813,7 +18813,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B6" s="8">
         <v>197</v>
@@ -18825,10 +18825,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G6" s="18">
         <v>380000</v>
@@ -18842,7 +18842,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B7" s="8">
         <v>198</v>
@@ -18854,10 +18854,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G7" s="18">
         <v>390000</v>
@@ -18871,7 +18871,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B8" s="8">
         <v>199</v>
@@ -18883,10 +18883,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G8" s="18">
         <v>400000</v>
@@ -18900,7 +18900,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B10" s="8">
         <v>200</v>
@@ -18912,10 +18912,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>560</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>562</v>
       </c>
       <c r="G10" s="18">
         <v>380000</v>
@@ -18929,7 +18929,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B11" s="8">
         <v>201</v>
@@ -18941,10 +18941,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G11" s="18">
         <v>400000</v>
@@ -18958,7 +18958,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B12" s="8">
         <v>202</v>
@@ -18970,7 +18970,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="18">
@@ -18985,7 +18985,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B13" s="8">
         <v>203</v>
@@ -18997,10 +18997,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G13" s="18">
         <v>385000</v>
@@ -19014,7 +19014,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B14" s="8">
         <v>204</v>
@@ -19026,10 +19026,10 @@
         <v>13</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G14" s="9">
         <v>410000</v>
@@ -19043,7 +19043,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B15" s="8">
         <v>205</v>
@@ -19055,10 +19055,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G15" s="14">
         <v>425000</v>
@@ -19072,7 +19072,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B16" s="8">
         <v>206</v>
@@ -19084,10 +19084,10 @@
         <v>13</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G16" s="14">
         <v>500000</v>
@@ -19101,12 +19101,12 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B18">
         <v>207</v>
@@ -19118,10 +19118,10 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F18" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G18" s="14">
         <v>395000</v>
@@ -19135,7 +19135,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B19">
         <v>208</v>
@@ -19147,10 +19147,10 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="G19" s="14">
         <v>400000</v>
@@ -19164,7 +19164,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B20">
         <v>209</v>
@@ -19176,10 +19176,10 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F20" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G20" s="14">
         <v>410000</v>
@@ -19193,7 +19193,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B21">
         <v>210</v>
@@ -19205,10 +19205,10 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F21" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G21" s="14">
         <v>415000</v>
@@ -19222,7 +19222,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B22">
         <v>211</v>
@@ -19234,7 +19234,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G22" s="14">
         <v>450000</v>
@@ -19259,7 +19259,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B25" s="9">
         <v>20</v>
@@ -19271,10 +19271,10 @@
         <v>48</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="G25" s="18">
         <v>1000000</v>
@@ -19288,7 +19288,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B26" s="19">
         <v>113</v>
@@ -19300,7 +19300,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="25">
@@ -19456,7 +19456,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B5" s="4">
         <v>47</v>
@@ -19468,10 +19468,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G5" s="20">
         <v>2000</v>
@@ -19630,7 +19630,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" s="15">
         <v>87</v>
@@ -19642,10 +19642,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G11" s="22">
         <v>500</v>
@@ -19659,7 +19659,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B12" s="15">
         <v>88</v>
@@ -19671,10 +19671,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G12" s="15">
         <v>500</v>
@@ -19688,7 +19688,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B13" s="15">
         <v>89</v>
@@ -19700,10 +19700,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G13" s="15">
         <v>500</v>
@@ -19717,7 +19717,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B14" s="15">
         <v>90</v>
@@ -19729,10 +19729,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G14" s="15">
         <v>500</v>
@@ -19746,7 +19746,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B15" s="15">
         <v>91</v>
@@ -19755,13 +19755,13 @@
         <v>90</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G15" s="15">
         <v>500</v>
@@ -19775,7 +19775,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B16" s="15">
         <v>92</v>
@@ -19787,10 +19787,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G16" s="15">
         <v>500</v>
@@ -19804,7 +19804,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B17" s="15">
         <v>93</v>
@@ -19816,10 +19816,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G17" s="15">
         <v>500</v>
@@ -19836,7 +19836,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B18" s="15">
         <v>94</v>
@@ -19848,10 +19848,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G18" s="15">
         <v>500</v>
@@ -19865,7 +19865,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B19" s="15">
         <v>117</v>
@@ -19877,10 +19877,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G19" s="15">
         <v>500</v>
@@ -19894,7 +19894,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B20" s="15">
         <v>118</v>
@@ -19906,10 +19906,10 @@
         <v>7</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G20" s="15">
         <v>1000</v>
@@ -19923,7 +19923,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B21" s="15">
         <v>119</v>
@@ -19935,10 +19935,10 @@
         <v>7</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G21" s="15">
         <v>1000</v>
@@ -19952,7 +19952,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B22" s="15">
         <v>175</v>
@@ -19964,10 +19964,10 @@
         <v>7</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G22" s="15">
         <v>1000</v>
@@ -19981,7 +19981,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B23" s="4">
         <v>176</v>
@@ -19993,10 +19993,10 @@
         <v>7</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G23" s="4">
         <v>1000</v>
@@ -20008,12 +20008,12 @@
         <v>200</v>
       </c>
       <c r="K23" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B24" s="4">
         <v>177</v>
@@ -20025,10 +20025,10 @@
         <v>7</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G24" s="4">
         <v>1000</v>
@@ -20040,12 +20040,12 @@
         <v>200</v>
       </c>
       <c r="K24" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B25" s="4">
         <v>178</v>
@@ -20057,10 +20057,10 @@
         <v>7</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G25" s="4">
         <v>1000</v>
@@ -20072,12 +20072,12 @@
         <v>200</v>
       </c>
       <c r="K25" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B26" s="4">
         <v>179</v>
@@ -20089,10 +20089,10 @@
         <v>7</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G26" s="4">
         <v>1000</v>
@@ -20106,7 +20106,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B27" s="4">
         <v>180</v>
@@ -20118,10 +20118,10 @@
         <v>7</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G27" s="4">
         <v>1000</v>
@@ -20135,7 +20135,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B28" s="4">
         <v>181</v>
@@ -20147,10 +20147,10 @@
         <v>7</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G28" s="4">
         <v>1000</v>
@@ -20164,7 +20164,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B29" s="4">
         <v>182</v>
@@ -20176,10 +20176,10 @@
         <v>7</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G29" s="4">
         <v>1000</v>
@@ -20193,7 +20193,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B30" s="4">
         <v>183</v>
@@ -20205,10 +20205,10 @@
         <v>7</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G30" s="4">
         <v>1500</v>
@@ -20222,7 +20222,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B31" s="15">
         <v>214</v>
@@ -20234,10 +20234,10 @@
         <v>7</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="G31" s="15">
         <v>500</v>
@@ -20251,7 +20251,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B32" s="15">
         <v>215</v>
@@ -20263,10 +20263,10 @@
         <v>7</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="G32" s="15">
         <v>500</v>
@@ -20280,7 +20280,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B33" s="15">
         <v>216</v>
@@ -20292,10 +20292,10 @@
         <v>7</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G33" s="15">
         <v>500</v>
@@ -20309,7 +20309,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B34" s="41">
         <v>217</v>
@@ -20321,10 +20321,10 @@
         <v>7</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G34" s="41">
         <v>1000</v>

</xml_diff>

<commit_message>
quest change and other small fixes
</commit_message>
<xml_diff>
--- a/Quests.xlsx
+++ b/Quests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754E1D56-BBDB-48BF-B9B9-BADB8C749589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4EF13C-8034-469D-9333-CFDA27A99A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="16440" tabRatio="680" activeTab="5" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="3210" yWindow="3825" windowWidth="25380" windowHeight="14985" tabRatio="680" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="619">
   <si>
     <t>Quest</t>
   </si>
@@ -1876,6 +1876,30 @@
   </si>
   <si>
     <t>Flame On!</t>
+  </si>
+  <si>
+    <t>Eight Legs</t>
+  </si>
+  <si>
+    <t>8 cave spiders</t>
+  </si>
+  <si>
+    <t>Double Double Toil And Trouble</t>
+  </si>
+  <si>
+    <t>3 witches</t>
+  </si>
+  <si>
+    <t>offhand of choice</t>
+  </si>
+  <si>
+    <t>chest of choice</t>
+  </si>
+  <si>
+    <t>weapon of choice</t>
+  </si>
+  <si>
+    <t>The Long Way</t>
   </si>
 </sst>
 </file>
@@ -13404,10 +13428,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13490,7 +13514,7 @@
         <v>474</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>617</v>
       </c>
       <c r="G3" s="18">
         <v>750</v>
@@ -14427,6 +14451,54 @@
       </c>
       <c r="I35" s="7">
         <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="G36" s="14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="G37" s="14">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>618</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="14">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -17591,8 +17663,8 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>